<commit_message>
Add able to load map with floors and walls.
</commit_message>
<xml_diff>
--- a/MapDesign_lvl1.xlsx
+++ b/MapDesign_lvl1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanyiecher\Desktop\SEMESTER_2\GameDev\Assignment2_GDT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanyiecher\Desktop\SEMESTER_2\SP3\SP3_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -164,7 +164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -350,6 +350,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -511,10 +517,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -839,7 +846,7 @@
   <dimension ref="A1:DY25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+      <selection activeCell="AA11" sqref="AA11:AA19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,80 +1062,80 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
-      <c r="AB2">
-        <v>0</v>
-      </c>
-      <c r="AC2">
-        <v>0</v>
-      </c>
-      <c r="AD2">
-        <v>0</v>
+      <c r="F2" s="3">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3">
+        <v>5</v>
+      </c>
+      <c r="I2" s="3">
+        <v>5</v>
+      </c>
+      <c r="J2" s="3">
+        <v>5</v>
+      </c>
+      <c r="K2" s="3">
+        <v>5</v>
+      </c>
+      <c r="L2" s="3">
+        <v>5</v>
+      </c>
+      <c r="M2" s="3">
+        <v>5</v>
+      </c>
+      <c r="N2" s="3">
+        <v>5</v>
+      </c>
+      <c r="O2" s="3">
+        <v>5</v>
+      </c>
+      <c r="P2" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>5</v>
+      </c>
+      <c r="R2" s="3">
+        <v>5</v>
+      </c>
+      <c r="S2" s="3">
+        <v>5</v>
+      </c>
+      <c r="T2" s="3">
+        <v>5</v>
+      </c>
+      <c r="U2" s="3">
+        <v>5</v>
+      </c>
+      <c r="V2" s="3">
+        <v>5</v>
+      </c>
+      <c r="W2" s="3">
+        <v>5</v>
+      </c>
+      <c r="X2" s="3">
+        <v>5</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>5</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>5</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>5</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>5</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>5</v>
+      </c>
+      <c r="AD2" s="3">
+        <v>5</v>
       </c>
       <c r="AE2">
         <v>0</v>
@@ -1250,8 +1257,8 @@
       <c r="E3" s="2">
         <v>0</v>
       </c>
-      <c r="F3" s="2">
-        <v>0</v>
+      <c r="F3" s="3">
+        <v>5</v>
       </c>
       <c r="G3" s="2">
         <v>0</v>
@@ -1322,8 +1329,8 @@
       <c r="AC3" s="2">
         <v>0</v>
       </c>
-      <c r="AD3" s="2">
-        <v>0</v>
+      <c r="AD3" s="3">
+        <v>5</v>
       </c>
       <c r="AE3" s="2">
         <v>0</v>
@@ -1445,8 +1452,8 @@
       <c r="E4" s="2">
         <v>0</v>
       </c>
-      <c r="F4" s="2">
-        <v>0</v>
+      <c r="F4" s="3">
+        <v>5</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
@@ -1517,8 +1524,8 @@
       <c r="AC4" s="2">
         <v>0</v>
       </c>
-      <c r="AD4" s="2">
-        <v>0</v>
+      <c r="AD4" s="3">
+        <v>5</v>
       </c>
       <c r="AE4" s="2">
         <v>0</v>
@@ -1640,8 +1647,8 @@
       <c r="E5" s="2">
         <v>0</v>
       </c>
-      <c r="F5" s="2">
-        <v>0</v>
+      <c r="F5" s="3">
+        <v>5</v>
       </c>
       <c r="G5" s="2">
         <v>0</v>
@@ -1712,8 +1719,8 @@
       <c r="AC5" s="2">
         <v>0</v>
       </c>
-      <c r="AD5" s="2">
-        <v>0</v>
+      <c r="AD5" s="3">
+        <v>5</v>
       </c>
       <c r="AE5" s="2">
         <v>0</v>
@@ -1835,8 +1842,8 @@
       <c r="E6" s="2">
         <v>0</v>
       </c>
-      <c r="F6" s="2">
-        <v>0</v>
+      <c r="F6" s="3">
+        <v>5</v>
       </c>
       <c r="G6" s="2">
         <v>0</v>
@@ -1907,8 +1914,8 @@
       <c r="AC6" s="2">
         <v>0</v>
       </c>
-      <c r="AD6" s="2">
-        <v>0</v>
+      <c r="AD6" s="3">
+        <v>5</v>
       </c>
       <c r="AE6" s="2">
         <v>0</v>
@@ -2030,8 +2037,8 @@
       <c r="E7" s="2">
         <v>0</v>
       </c>
-      <c r="F7" s="2">
-        <v>0</v>
+      <c r="F7" s="3">
+        <v>5</v>
       </c>
       <c r="G7" s="2">
         <v>0</v>
@@ -2102,8 +2109,8 @@
       <c r="AC7" s="2">
         <v>0</v>
       </c>
-      <c r="AD7" s="2">
-        <v>0</v>
+      <c r="AD7" s="3">
+        <v>5</v>
       </c>
       <c r="AE7" s="2">
         <v>0</v>
@@ -2225,8 +2232,8 @@
       <c r="E8" s="2">
         <v>0</v>
       </c>
-      <c r="F8" s="2">
-        <v>0</v>
+      <c r="F8" s="3">
+        <v>5</v>
       </c>
       <c r="G8" s="2">
         <v>0</v>
@@ -2297,8 +2304,8 @@
       <c r="AC8" s="2">
         <v>0</v>
       </c>
-      <c r="AD8" s="2">
-        <v>0</v>
+      <c r="AD8" s="3">
+        <v>5</v>
       </c>
       <c r="AE8" s="2">
         <v>0</v>
@@ -2420,8 +2427,8 @@
       <c r="E9" s="2">
         <v>0</v>
       </c>
-      <c r="F9" s="2">
-        <v>0</v>
+      <c r="F9" s="3">
+        <v>5</v>
       </c>
       <c r="G9" s="2">
         <v>0</v>
@@ -2441,8 +2448,8 @@
       <c r="L9" s="2">
         <v>0</v>
       </c>
-      <c r="M9" s="2">
-        <v>0</v>
+      <c r="M9" s="3">
+        <v>5</v>
       </c>
       <c r="N9" s="2">
         <v>0</v>
@@ -2462,8 +2469,8 @@
       <c r="S9" s="2">
         <v>0</v>
       </c>
-      <c r="T9" s="2">
-        <v>0</v>
+      <c r="T9" s="3">
+        <v>5</v>
       </c>
       <c r="U9" s="2">
         <v>0</v>
@@ -2471,8 +2478,8 @@
       <c r="V9" s="2">
         <v>0</v>
       </c>
-      <c r="W9" s="2">
-        <v>0</v>
+      <c r="W9" s="3">
+        <v>5</v>
       </c>
       <c r="X9" s="2">
         <v>0</v>
@@ -2492,8 +2499,8 @@
       <c r="AC9" s="2">
         <v>0</v>
       </c>
-      <c r="AD9" s="2">
-        <v>0</v>
+      <c r="AD9" s="3">
+        <v>5</v>
       </c>
       <c r="AE9" s="2">
         <v>0</v>
@@ -2615,8 +2622,8 @@
       <c r="E10" s="2">
         <v>0</v>
       </c>
-      <c r="F10" s="2">
-        <v>0</v>
+      <c r="F10" s="3">
+        <v>5</v>
       </c>
       <c r="G10" s="2">
         <v>0</v>
@@ -2636,8 +2643,8 @@
       <c r="L10" s="2">
         <v>0</v>
       </c>
-      <c r="M10" s="2">
-        <v>0</v>
+      <c r="M10" s="3">
+        <v>5</v>
       </c>
       <c r="N10" s="2">
         <v>0</v>
@@ -2657,8 +2664,8 @@
       <c r="S10" s="2">
         <v>0</v>
       </c>
-      <c r="T10" s="2">
-        <v>0</v>
+      <c r="T10" s="3">
+        <v>5</v>
       </c>
       <c r="U10" s="2">
         <v>0</v>
@@ -2666,8 +2673,8 @@
       <c r="V10" s="2">
         <v>0</v>
       </c>
-      <c r="W10" s="2">
-        <v>0</v>
+      <c r="W10" s="3">
+        <v>5</v>
       </c>
       <c r="X10" s="2">
         <v>0</v>
@@ -2687,8 +2694,8 @@
       <c r="AC10" s="2">
         <v>0</v>
       </c>
-      <c r="AD10" s="2">
-        <v>0</v>
+      <c r="AD10" s="3">
+        <v>5</v>
       </c>
       <c r="AE10" s="2">
         <v>0</v>
@@ -2810,8 +2817,8 @@
       <c r="E11" s="2">
         <v>0</v>
       </c>
-      <c r="F11" s="2">
-        <v>0</v>
+      <c r="F11" s="3">
+        <v>5</v>
       </c>
       <c r="G11" s="2">
         <v>0</v>
@@ -2831,8 +2838,8 @@
       <c r="L11" s="2">
         <v>0</v>
       </c>
-      <c r="M11" s="2">
-        <v>0</v>
+      <c r="M11" s="3">
+        <v>5</v>
       </c>
       <c r="N11" s="2">
         <v>0</v>
@@ -2852,8 +2859,8 @@
       <c r="S11" s="2">
         <v>0</v>
       </c>
-      <c r="T11" s="2">
-        <v>0</v>
+      <c r="T11" s="3">
+        <v>5</v>
       </c>
       <c r="U11" s="2">
         <v>0</v>
@@ -2861,8 +2868,8 @@
       <c r="V11" s="2">
         <v>0</v>
       </c>
-      <c r="W11" s="2">
-        <v>0</v>
+      <c r="W11" s="3">
+        <v>5</v>
       </c>
       <c r="X11" s="2">
         <v>0</v>
@@ -2873,8 +2880,8 @@
       <c r="Z11" s="2">
         <v>0</v>
       </c>
-      <c r="AA11" s="2">
-        <v>0</v>
+      <c r="AA11" s="3">
+        <v>5</v>
       </c>
       <c r="AB11" s="2">
         <v>0</v>
@@ -2882,8 +2889,8 @@
       <c r="AC11" s="2">
         <v>0</v>
       </c>
-      <c r="AD11" s="2">
-        <v>0</v>
+      <c r="AD11" s="3">
+        <v>5</v>
       </c>
       <c r="AE11" s="2">
         <v>0</v>
@@ -3005,8 +3012,8 @@
       <c r="E12" s="2">
         <v>0</v>
       </c>
-      <c r="F12" s="2">
-        <v>0</v>
+      <c r="F12" s="3">
+        <v>5</v>
       </c>
       <c r="G12" s="2">
         <v>0</v>
@@ -3026,8 +3033,8 @@
       <c r="L12" s="2">
         <v>0</v>
       </c>
-      <c r="M12" s="2">
-        <v>0</v>
+      <c r="M12" s="3">
+        <v>5</v>
       </c>
       <c r="N12" s="2">
         <v>0</v>
@@ -3047,8 +3054,8 @@
       <c r="S12" s="2">
         <v>0</v>
       </c>
-      <c r="T12" s="2">
-        <v>0</v>
+      <c r="T12" s="3">
+        <v>5</v>
       </c>
       <c r="U12" s="2">
         <v>0</v>
@@ -3056,8 +3063,8 @@
       <c r="V12" s="2">
         <v>0</v>
       </c>
-      <c r="W12" s="2">
-        <v>0</v>
+      <c r="W12" s="3">
+        <v>5</v>
       </c>
       <c r="X12" s="2">
         <v>0</v>
@@ -3068,8 +3075,8 @@
       <c r="Z12" s="2">
         <v>0</v>
       </c>
-      <c r="AA12" s="2">
-        <v>0</v>
+      <c r="AA12" s="3">
+        <v>5</v>
       </c>
       <c r="AB12" s="2">
         <v>0</v>
@@ -3077,8 +3084,8 @@
       <c r="AC12" s="2">
         <v>0</v>
       </c>
-      <c r="AD12" s="2">
-        <v>0</v>
+      <c r="AD12" s="3">
+        <v>5</v>
       </c>
       <c r="AE12" s="2">
         <v>0</v>
@@ -3200,8 +3207,8 @@
       <c r="E13" s="2">
         <v>0</v>
       </c>
-      <c r="F13" s="2">
-        <v>0</v>
+      <c r="F13" s="3">
+        <v>5</v>
       </c>
       <c r="G13" s="2">
         <v>0</v>
@@ -3221,8 +3228,8 @@
       <c r="L13" s="2">
         <v>0</v>
       </c>
-      <c r="M13" s="2">
-        <v>0</v>
+      <c r="M13" s="3">
+        <v>5</v>
       </c>
       <c r="N13" s="2">
         <v>0</v>
@@ -3242,8 +3249,8 @@
       <c r="S13" s="2">
         <v>0</v>
       </c>
-      <c r="T13" s="2">
-        <v>0</v>
+      <c r="T13" s="3">
+        <v>5</v>
       </c>
       <c r="U13" s="2">
         <v>0</v>
@@ -3251,8 +3258,8 @@
       <c r="V13" s="2">
         <v>0</v>
       </c>
-      <c r="W13" s="2">
-        <v>0</v>
+      <c r="W13" s="3">
+        <v>5</v>
       </c>
       <c r="X13" s="2">
         <v>0</v>
@@ -3263,8 +3270,8 @@
       <c r="Z13" s="2">
         <v>0</v>
       </c>
-      <c r="AA13" s="2">
-        <v>0</v>
+      <c r="AA13" s="3">
+        <v>5</v>
       </c>
       <c r="AB13" s="2">
         <v>0</v>
@@ -3272,8 +3279,8 @@
       <c r="AC13" s="2">
         <v>0</v>
       </c>
-      <c r="AD13" s="2">
-        <v>0</v>
+      <c r="AD13" s="3">
+        <v>5</v>
       </c>
       <c r="AE13" s="2">
         <v>0</v>
@@ -3395,8 +3402,8 @@
       <c r="E14" s="2">
         <v>0</v>
       </c>
-      <c r="F14" s="2">
-        <v>0</v>
+      <c r="F14" s="3">
+        <v>5</v>
       </c>
       <c r="G14" s="2">
         <v>0</v>
@@ -3416,8 +3423,8 @@
       <c r="L14" s="2">
         <v>0</v>
       </c>
-      <c r="M14" s="2">
-        <v>0</v>
+      <c r="M14" s="3">
+        <v>5</v>
       </c>
       <c r="N14" s="2">
         <v>0</v>
@@ -3437,8 +3444,8 @@
       <c r="S14" s="2">
         <v>0</v>
       </c>
-      <c r="T14" s="2">
-        <v>0</v>
+      <c r="T14" s="3">
+        <v>5</v>
       </c>
       <c r="U14" s="2">
         <v>0</v>
@@ -3446,8 +3453,8 @@
       <c r="V14" s="2">
         <v>0</v>
       </c>
-      <c r="W14" s="2">
-        <v>0</v>
+      <c r="W14" s="3">
+        <v>5</v>
       </c>
       <c r="X14" s="2">
         <v>0</v>
@@ -3458,8 +3465,8 @@
       <c r="Z14" s="2">
         <v>0</v>
       </c>
-      <c r="AA14" s="2">
-        <v>0</v>
+      <c r="AA14" s="3">
+        <v>5</v>
       </c>
       <c r="AB14" s="2">
         <v>0</v>
@@ -3467,8 +3474,8 @@
       <c r="AC14" s="2">
         <v>0</v>
       </c>
-      <c r="AD14" s="2">
-        <v>0</v>
+      <c r="AD14" s="3">
+        <v>5</v>
       </c>
       <c r="AE14" s="2">
         <v>0</v>
@@ -3590,8 +3597,8 @@
       <c r="E15" s="2">
         <v>0</v>
       </c>
-      <c r="F15" s="2">
-        <v>0</v>
+      <c r="F15" s="3">
+        <v>5</v>
       </c>
       <c r="G15" s="2">
         <v>0</v>
@@ -3611,8 +3618,8 @@
       <c r="L15" s="2">
         <v>0</v>
       </c>
-      <c r="M15" s="2">
-        <v>0</v>
+      <c r="M15" s="3">
+        <v>5</v>
       </c>
       <c r="N15" s="2">
         <v>0</v>
@@ -3632,8 +3639,8 @@
       <c r="S15" s="2">
         <v>0</v>
       </c>
-      <c r="T15" s="2">
-        <v>0</v>
+      <c r="T15" s="3">
+        <v>5</v>
       </c>
       <c r="U15" s="2">
         <v>0</v>
@@ -3641,8 +3648,8 @@
       <c r="V15" s="2">
         <v>0</v>
       </c>
-      <c r="W15" s="2">
-        <v>0</v>
+      <c r="W15" s="3">
+        <v>5</v>
       </c>
       <c r="X15" s="2">
         <v>0</v>
@@ -3653,8 +3660,8 @@
       <c r="Z15" s="2">
         <v>0</v>
       </c>
-      <c r="AA15" s="2">
-        <v>0</v>
+      <c r="AA15" s="3">
+        <v>5</v>
       </c>
       <c r="AB15" s="2">
         <v>0</v>
@@ -3662,8 +3669,8 @@
       <c r="AC15" s="2">
         <v>0</v>
       </c>
-      <c r="AD15" s="2">
-        <v>0</v>
+      <c r="AD15" s="3">
+        <v>5</v>
       </c>
       <c r="AE15" s="2">
         <v>0</v>
@@ -3785,8 +3792,8 @@
       <c r="E16" s="2">
         <v>0</v>
       </c>
-      <c r="F16" s="2">
-        <v>0</v>
+      <c r="F16" s="3">
+        <v>5</v>
       </c>
       <c r="G16" s="2">
         <v>0</v>
@@ -3806,8 +3813,8 @@
       <c r="L16" s="2">
         <v>0</v>
       </c>
-      <c r="M16" s="2">
-        <v>0</v>
+      <c r="M16" s="3">
+        <v>5</v>
       </c>
       <c r="N16" s="2">
         <v>0</v>
@@ -3827,8 +3834,8 @@
       <c r="S16" s="2">
         <v>0</v>
       </c>
-      <c r="T16" s="2">
-        <v>0</v>
+      <c r="T16" s="3">
+        <v>5</v>
       </c>
       <c r="U16" s="2">
         <v>0</v>
@@ -3836,8 +3843,8 @@
       <c r="V16" s="2">
         <v>0</v>
       </c>
-      <c r="W16" s="2">
-        <v>0</v>
+      <c r="W16" s="3">
+        <v>5</v>
       </c>
       <c r="X16" s="2">
         <v>0</v>
@@ -3848,8 +3855,8 @@
       <c r="Z16" s="2">
         <v>0</v>
       </c>
-      <c r="AA16" s="2">
-        <v>0</v>
+      <c r="AA16" s="3">
+        <v>5</v>
       </c>
       <c r="AB16" s="2">
         <v>0</v>
@@ -3857,8 +3864,8 @@
       <c r="AC16" s="2">
         <v>0</v>
       </c>
-      <c r="AD16" s="2">
-        <v>0</v>
+      <c r="AD16" s="3">
+        <v>5</v>
       </c>
       <c r="AE16" s="2">
         <v>0</v>
@@ -3980,8 +3987,8 @@
       <c r="E17" s="2">
         <v>0</v>
       </c>
-      <c r="F17" s="2">
-        <v>0</v>
+      <c r="F17" s="3">
+        <v>5</v>
       </c>
       <c r="G17" s="2">
         <v>0</v>
@@ -4001,8 +4008,8 @@
       <c r="L17" s="2">
         <v>0</v>
       </c>
-      <c r="M17" s="2">
-        <v>0</v>
+      <c r="M17" s="3">
+        <v>5</v>
       </c>
       <c r="N17" s="2">
         <v>0</v>
@@ -4022,8 +4029,8 @@
       <c r="S17" s="2">
         <v>0</v>
       </c>
-      <c r="T17" s="2">
-        <v>0</v>
+      <c r="T17" s="3">
+        <v>5</v>
       </c>
       <c r="U17" s="2">
         <v>0</v>
@@ -4043,8 +4050,8 @@
       <c r="Z17" s="2">
         <v>0</v>
       </c>
-      <c r="AA17" s="2">
-        <v>0</v>
+      <c r="AA17" s="3">
+        <v>5</v>
       </c>
       <c r="AB17" s="2">
         <v>0</v>
@@ -4052,8 +4059,8 @@
       <c r="AC17" s="2">
         <v>0</v>
       </c>
-      <c r="AD17" s="2">
-        <v>0</v>
+      <c r="AD17" s="3">
+        <v>5</v>
       </c>
       <c r="AE17" s="2">
         <v>0</v>
@@ -4175,8 +4182,8 @@
       <c r="E18" s="2">
         <v>0</v>
       </c>
-      <c r="F18" s="2">
-        <v>0</v>
+      <c r="F18" s="3">
+        <v>5</v>
       </c>
       <c r="G18" s="2">
         <v>0</v>
@@ -4199,23 +4206,23 @@
       <c r="M18" s="2">
         <v>0</v>
       </c>
-      <c r="N18" s="2">
-        <v>0</v>
-      </c>
-      <c r="O18" s="2">
-        <v>0</v>
-      </c>
-      <c r="P18" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="2">
-        <v>0</v>
-      </c>
-      <c r="R18" s="2">
-        <v>0</v>
-      </c>
-      <c r="S18" s="2">
-        <v>0</v>
+      <c r="N18" s="3">
+        <v>5</v>
+      </c>
+      <c r="O18" s="3">
+        <v>5</v>
+      </c>
+      <c r="P18" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>5</v>
+      </c>
+      <c r="R18" s="3">
+        <v>5</v>
+      </c>
+      <c r="S18" s="3">
+        <v>5</v>
       </c>
       <c r="T18" s="2">
         <v>0</v>
@@ -4238,8 +4245,8 @@
       <c r="Z18" s="2">
         <v>0</v>
       </c>
-      <c r="AA18" s="2">
-        <v>0</v>
+      <c r="AA18" s="3">
+        <v>5</v>
       </c>
       <c r="AB18" s="2">
         <v>0</v>
@@ -4247,8 +4254,8 @@
       <c r="AC18" s="2">
         <v>0</v>
       </c>
-      <c r="AD18" s="2">
-        <v>0</v>
+      <c r="AD18" s="3">
+        <v>5</v>
       </c>
       <c r="AE18" s="2">
         <v>0</v>
@@ -4370,8 +4377,8 @@
       <c r="E19" s="2">
         <v>0</v>
       </c>
-      <c r="F19" s="2">
-        <v>0</v>
+      <c r="F19" s="3">
+        <v>5</v>
       </c>
       <c r="G19" s="2">
         <v>0</v>
@@ -4433,8 +4440,8 @@
       <c r="Z19" s="2">
         <v>0</v>
       </c>
-      <c r="AA19" s="2">
-        <v>0</v>
+      <c r="AA19" s="3">
+        <v>5</v>
       </c>
       <c r="AB19" s="2">
         <v>0</v>
@@ -4442,8 +4449,8 @@
       <c r="AC19" s="2">
         <v>0</v>
       </c>
-      <c r="AD19" s="2">
-        <v>0</v>
+      <c r="AD19" s="3">
+        <v>5</v>
       </c>
       <c r="AE19" s="2">
         <v>0</v>
@@ -4565,8 +4572,8 @@
       <c r="E20" s="2">
         <v>0</v>
       </c>
-      <c r="F20" s="2">
-        <v>0</v>
+      <c r="F20" s="3">
+        <v>5</v>
       </c>
       <c r="G20" s="2">
         <v>0</v>
@@ -4637,8 +4644,8 @@
       <c r="AC20" s="2">
         <v>0</v>
       </c>
-      <c r="AD20" s="2">
-        <v>0</v>
+      <c r="AD20" s="3">
+        <v>5</v>
       </c>
       <c r="AE20" s="2">
         <v>0</v>
@@ -4760,8 +4767,8 @@
       <c r="E21" s="2">
         <v>0</v>
       </c>
-      <c r="F21" s="2">
-        <v>0</v>
+      <c r="F21" s="3">
+        <v>5</v>
       </c>
       <c r="G21" s="2">
         <v>0</v>
@@ -4832,8 +4839,8 @@
       <c r="AC21" s="2">
         <v>0</v>
       </c>
-      <c r="AD21" s="2">
-        <v>0</v>
+      <c r="AD21" s="3">
+        <v>5</v>
       </c>
       <c r="AE21" s="2">
         <v>0</v>
@@ -4955,8 +4962,8 @@
       <c r="E22" s="2">
         <v>0</v>
       </c>
-      <c r="F22" s="2">
-        <v>0</v>
+      <c r="F22" s="3">
+        <v>5</v>
       </c>
       <c r="G22" s="2">
         <v>0</v>
@@ -5027,8 +5034,8 @@
       <c r="AC22" s="2">
         <v>0</v>
       </c>
-      <c r="AD22" s="2">
-        <v>0</v>
+      <c r="AD22" s="3">
+        <v>5</v>
       </c>
       <c r="AE22" s="2">
         <v>0</v>
@@ -5150,8 +5157,8 @@
       <c r="E23" s="2">
         <v>0</v>
       </c>
-      <c r="F23" s="2">
-        <v>0</v>
+      <c r="F23" s="3">
+        <v>5</v>
       </c>
       <c r="G23" s="2">
         <v>0</v>
@@ -5222,8 +5229,8 @@
       <c r="AC23" s="2">
         <v>0</v>
       </c>
-      <c r="AD23" s="2">
-        <v>0</v>
+      <c r="AD23" s="3">
+        <v>5</v>
       </c>
       <c r="AE23" s="2">
         <v>0</v>

</xml_diff>